<commit_message>
moving range of cells
</commit_message>
<xml_diff>
--- a/openpyxl/Doc_Excel.xlsx
+++ b/openpyxl/Doc_Excel.xlsx
@@ -133,7 +133,7 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>1</col>
+      <col>7</col>
       <colOff>0</colOff>
       <row>5</row>
       <rowOff>0</rowOff>
@@ -482,10 +482,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="C4" t="n">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <f>SUM(A2, A4)</f>
         <v/>
       </c>
@@ -507,19 +507,14 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-    </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -534,6 +529,9 @@
         </is>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>

</xml_diff>